<commit_message>
working on complete the attendance report for both instructors and student
</commit_message>
<xml_diff>
--- a/AttendenceSystem/AttendenceSystem/wwwroot/ExcelTemplate/UploadBulkStudent.xlsx
+++ b/AttendenceSystem/AttendenceSystem/wwwroot/ExcelTemplate/UploadBulkStudent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sherif\Desktop\MVC Project\MVC-Attendance-Project\AttendenceSystem\AttendenceSystem\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sherif\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25DCF1-71A4-41C5-B5A6-01F65C0C1570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5025E86D-23C3-4099-812B-5FBF052179FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{963AD9D3-5510-4B0B-BE7C-A5707723DCD0}"/>
+    <workbookView xWindow="4380" yWindow="1140" windowWidth="17280" windowHeight="8964" xr2:uid="{963AD9D3-5510-4B0B-BE7C-A5707723DCD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>University</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TrackId</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2535648-7E48-454D-A6D8-261C8AD9D5C2}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -452,9 +458,10 @@
     <col min="3" max="3" width="19.3984375" customWidth="1"/>
     <col min="6" max="6" width="19.19921875" customWidth="1"/>
     <col min="7" max="7" width="20.19921875" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,8 +486,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>

</xml_diff>